<commit_message>
Cleaned up, commented, checked E1 analyses
</commit_message>
<xml_diff>
--- a/Adult - Single Distractor/Results SD8-9-12.xlsx
+++ b/Adult - Single Distractor/Results SD8-9-12.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -317,11 +317,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2137236072"/>
-        <c:axId val="2137239048"/>
+        <c:axId val="2087496552"/>
+        <c:axId val="2087499528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2137236072"/>
+        <c:axId val="2087496552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -330,7 +330,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2137239048"/>
+        <c:crossAx val="2087499528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -338,7 +338,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2137239048"/>
+        <c:axId val="2087499528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -373,7 +373,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2137236072"/>
+        <c:crossAx val="2087496552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -621,11 +621,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2090216216"/>
-        <c:axId val="2137191576"/>
+        <c:axId val="2127617880"/>
+        <c:axId val="2127614888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2090216216"/>
+        <c:axId val="2127617880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -634,7 +634,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2137191576"/>
+        <c:crossAx val="2127614888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -642,7 +642,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2137191576"/>
+        <c:axId val="2127614888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -677,7 +677,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090216216"/>
+        <c:crossAx val="2127617880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1056,7 +1056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>

</xml_diff>